<commit_message>
Made one minor edit on the “General Notes” tab for the surrogate key to indicate it as a sequential integer with no special meaning.
git-svn-id: https://omb-dashboardplatform.reisys.com:10039/NYC_Checkbook_2_0/Database@21 948744eb-f611-4f28-8820-250fb6d8f47d

Former-commit-id: 4ee2396e829e623deb0e9d338907173c536cfcff
</commit_message>
<xml_diff>
--- a/checkbook/Data Model/DataDictionary.xlsx
+++ b/checkbook/Data Model/DataDictionary.xlsx
@@ -50,8 +50,8 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Kishore K. Vuppala - Personal View" guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1916" windowHeight="815" activeSheetId="1"/>
     <customWorkbookView name="athiagarajan - Personal View" guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1916" windowHeight="815" activeSheetId="1"/>
-    <customWorkbookView name="Kishore K. Vuppala - Personal View" guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1916" windowHeight="815" activeSheetId="11"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -70,7 +70,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>athiagarajan:</t>
         </r>
@@ -79,7 +79,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Name of the Table</t>
@@ -94,7 +94,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>athiagarajan:</t>
         </r>
@@ -103,7 +103,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Indicates the domain name like Payroll, Contracts etc</t>
@@ -118,7 +118,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>athiagarajan:</t>
         </r>
@@ -127,7 +127,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Brief description on what kind of data is stored in the table</t>
@@ -142,7 +142,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>athiagarajan:</t>
         </r>
@@ -151,7 +151,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Heap table (Default) or Append only  table or compressed table
@@ -7825,7 +7825,7 @@
       </rPr>
       <t>" tables will include all documents as is irrespective of the visibility.
 Refer to the "Tables" worksheet for the list of these tables.
-Primary key which is used to identify a record uniquely is mostly kept as a surrogate key which is a meaningless integer. 
+Primary key which is used to identify a record uniquely is mostly kept as a surrogate key which is a sequential integer without any special meaning.  
 Such a key if provided by the source is made use of rather than generating another one. Alternate keys are column(s) other than primary key which are used to identify a record uniquely.
 These are also mentioned against each table in "Tables" worksheet.</t>
     </r>
@@ -7835,7 +7835,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="17">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7855,26 +7855,6 @@
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -7883,6 +7863,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -8029,38 +8016,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -8068,65 +8055,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8139,7 +8126,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{80270172-B507-4181-99B9-03E95E51C98B}" diskRevisions="1" revisionId="465" version="41">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{754A6DE8-7709-4C95-B37B-91AE37BE3170}" diskRevisions="1" revisionId="484" version="43">
   <header guid="{AB9580D8-241A-4669-9392-73D842CA78E7}" dateTime="2011-11-16T16:02:32" maxSheetId="12" userName="Kishore K. Vuppala" r:id="rId1">
     <sheetIdMap count="11">
       <sheetId val="1"/>
@@ -8755,49 +8742,79 @@
       <sheetId val="11"/>
     </sheetIdMap>
   </header>
+  <header guid="{5CFAD47E-E90B-4B05-9A84-4133AD3C3B70}" dateTime="2011-11-21T18:45:15" maxSheetId="12" userName="Kishore K. Vuppala" r:id="rId42" minRId="466">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="9"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{754A6DE8-7709-4C95-B37B-91AE37BE3170}" dateTime="2011-11-21T18:47:24" maxSheetId="12" userName="Kishore K. Vuppala" r:id="rId43">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="9"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcv guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+  <rcv guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>Tables!$A$2:$E$89</formula>
     <oldFormula>Tables!$A$2:$E$89</oldFormula>
   </rdn>
-  <rdn rId="0" localSheetId="3" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+  <rdn rId="0" localSheetId="3" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>'Chart of Accounts'!$A$3:$M$170</formula>
     <oldFormula>'Chart of Accounts'!$A$3:$M$170</oldFormula>
   </rdn>
-  <rdn rId="0" localSheetId="4" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+  <rdn rId="0" localSheetId="4" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>Vendor!$A$3:$M$45</formula>
     <oldFormula>Vendor!$A$3:$M$45</oldFormula>
   </rdn>
-  <rdn rId="0" localSheetId="5" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+  <rdn rId="0" localSheetId="5" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>Contracts!$A$4:$M$159</formula>
     <oldFormula>Contracts!$A$4:$M$159</oldFormula>
   </rdn>
-  <rdn rId="0" localSheetId="6" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+  <rdn rId="0" localSheetId="6" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>Disbursement!$A$3:$M$45</formula>
     <oldFormula>Disbursement!$A$3:$M$45</oldFormula>
   </rdn>
-  <rdn rId="0" localSheetId="7" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+  <rdn rId="0" localSheetId="7" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>Budget!$A$3:$M$21</formula>
     <oldFormula>Budget!$A$3:$M$21</oldFormula>
   </rdn>
-  <rdn rId="0" localSheetId="8" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+  <rdn rId="0" localSheetId="8" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>Revenue!$A$3:$M$76</formula>
     <oldFormula>Revenue!$A$3:$M$76</oldFormula>
   </rdn>
-  <rdn rId="0" localSheetId="10" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+  <rdn rId="0" localSheetId="10" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>'Reference Tables'!$A$3:$M$140</formula>
     <oldFormula>'Reference Tables'!$A$3:$M$140</oldFormula>
   </rdn>
-  <rdn rId="0" localSheetId="11" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+  <rdn rId="0" localSheetId="11" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>'Fact Tables'!$A$3:$M$3</formula>
     <oldFormula>'Fact Tables'!$A$3:$M$3</oldFormula>
   </rdn>
-  <rcv guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" action="add"/>
+  <rcv guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" action="add"/>
 </revisions>
 </file>
 
@@ -10337,6 +10354,241 @@
 
 <file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="466" sId="1">
+    <oc r="A1" t="inlineStr">
+      <is>
+        <r>
+          <t>Data dictionary provides a detailed coverage of all tables used by NYC Checkbook2.0 application.
+Information is organized in several worksheets. 
+- First is the list of all tables with the information on what kind of data is stored, subject area/domain to 
+  which it belongs to and the column(s) which can act as alternate/unique keys to identify a record uniquely.
+- Domains which are included are Chart of Accounts(COA), Vendor(FMSV), Contracts(CON &amp; MAG),
+Disbursement(FMS), Budget, Revenue, Payroll (PMS) and finally the reference tables.
+As NYC Checkbook considers only the latest version of contracts and disbursement, which are made available to the public as is or with some masking
+for security reasons, few additional tables are created. These tables have the prefix as either "</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>history_</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>" or "</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>all_</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>".
+"</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>History_</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>" tables will have all the versions of the document. "</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>All_</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>" tables will include all documents as is irrespective of the visibility.
+Refer to the "Tables" worksheet for the list of these tables.
+Primary key which is used to identify a record uniquely is mostly kept as a surrogate key which is a meaningless integer. 
+Such a key if provided by the source is made use of rather than generating another one. Alternate keys are column(s) other than primary key which are used to identify a record uniquely.
+These are also mentioned against each table in "Tables" worksheet.</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="A1" t="inlineStr">
+      <is>
+        <r>
+          <t>Data dictionary provides a detailed coverage of all tables used by NYC Checkbook2.0 application.
+Information is organized in several worksheets. 
+- First is the list of all tables with the information on what kind of data is stored, subject area/domain to 
+  which it belongs to and the column(s) which can act as alternate/unique keys to identify a record uniquely.
+- Domains which are included are Chart of Accounts(COA), Vendor(FMSV), Contracts(CON &amp; MAG),
+Disbursement(FMS), Budget, Revenue, Payroll (PMS) and finally the reference tables.
+As NYC Checkbook considers only the latest version of contracts and disbursement, which are made available to the public as is or with some masking
+for security reasons, few additional tables are created. These tables have the prefix as either "</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>history_</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>" or "</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>all_</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>".
+"</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>History_</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>" tables will have all the versions of the document. "</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>All_</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF0070C0"/>
+            <rFont val="Cambria"/>
+            <family val="1"/>
+          </rPr>
+          <t>" tables will include all documents as is irrespective of the visibility.
+Refer to the "Tables" worksheet for the list of these tables.
+Primary key which is used to identify a record uniquely is mostly kept as a surrogate key which is a sequential integer without any special meaning.  
+Such a key if provided by the source is made use of rather than generating another one. Alternate keys are column(s) other than primary key which are used to identify a record uniquely.
+These are also mentioned against each table in "Tables" worksheet.</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Tables!$A$2:$E$89</formula>
+    <oldFormula>Tables!$A$2:$E$89</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="3" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>'Chart of Accounts'!$A$3:$M$170</formula>
+    <oldFormula>'Chart of Accounts'!$A$3:$M$170</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="4" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Vendor!$A$3:$M$45</formula>
+    <oldFormula>Vendor!$A$3:$M$45</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="5" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Contracts!$A$4:$M$159</formula>
+    <oldFormula>Contracts!$A$4:$M$159</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="6" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Disbursement!$A$3:$M$45</formula>
+    <oldFormula>Disbursement!$A$3:$M$45</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="7" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Budget!$A$3:$M$21</formula>
+    <oldFormula>Budget!$A$3:$M$21</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="8" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Revenue!$A$3:$M$76</formula>
+    <oldFormula>Revenue!$A$3:$M$76</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="10" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>'Reference Tables'!$A$3:$M$140</formula>
+    <oldFormula>'Reference Tables'!$A$3:$M$140</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="11" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>'Fact Tables'!$A$3:$M$3</formula>
+    <oldFormula>'Fact Tables'!$A$3:$M$3</oldFormula>
+  </rdn>
+  <rcv guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog161.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rrc rId="309" sId="2" ref="A19:XFD19" action="insertRow"/>
   <rcc rId="310" sId="2">
     <nc r="B19" t="inlineStr">
@@ -10414,7 +10666,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog161.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog1611.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rcv guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" action="delete"/>
   <rdn rId="0" localSheetId="2" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
@@ -10454,49 +10706,6 @@
     <oldFormula>'Fact Tables'!$A$3:$M$3</oldFormula>
   </rdn>
   <rcv guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog1611.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcv guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>Tables!$A$2:$E$72</formula>
-    <oldFormula>Tables!$A$2:$E$72</oldFormula>
-  </rdn>
-  <rdn rId="0" localSheetId="3" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>'Chart of Accounts'!$A$3:$M$170</formula>
-    <oldFormula>'Chart of Accounts'!$A$3:$M$170</oldFormula>
-  </rdn>
-  <rdn rId="0" localSheetId="4" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>Vendor!$A$3:$M$45</formula>
-    <oldFormula>Vendor!$A$3:$M$45</oldFormula>
-  </rdn>
-  <rdn rId="0" localSheetId="5" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>Contracts!$A$4:$M$159</formula>
-    <oldFormula>Contracts!$A$4:$M$159</oldFormula>
-  </rdn>
-  <rdn rId="0" localSheetId="6" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>Disbursement!$A$3:$M$45</formula>
-    <oldFormula>Disbursement!$A$3:$M$45</oldFormula>
-  </rdn>
-  <rdn rId="0" localSheetId="7" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>Budget!$A$3:$M$21</formula>
-    <oldFormula>Budget!$A$3:$M$21</oldFormula>
-  </rdn>
-  <rdn rId="0" localSheetId="8" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>Revenue!$A$3:$M$76</formula>
-    <oldFormula>Revenue!$A$3:$M$76</oldFormula>
-  </rdn>
-  <rdn rId="0" localSheetId="10" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>'Reference Tables'!$A$3:$M$140</formula>
-    <oldFormula>'Reference Tables'!$A$3:$M$140</oldFormula>
-  </rdn>
-  <rdn rId="0" localSheetId="11" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>'Fact Tables'!$A$3:$M$3</formula>
-    <oldFormula>'Fact Tables'!$A$3:$M$3</oldFormula>
-  </rdn>
-  <rcv guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" action="add"/>
 </revisions>
 </file>
 
@@ -10544,6 +10753,49 @@
 </file>
 
 <file path=xl/revisions/revisionLog161111.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcv guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Tables!$A$2:$E$72</formula>
+    <oldFormula>Tables!$A$2:$E$72</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="3" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>'Chart of Accounts'!$A$3:$M$170</formula>
+    <oldFormula>'Chart of Accounts'!$A$3:$M$170</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="4" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Vendor!$A$3:$M$45</formula>
+    <oldFormula>Vendor!$A$3:$M$45</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="5" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Contracts!$A$4:$M$159</formula>
+    <oldFormula>Contracts!$A$4:$M$159</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="6" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Disbursement!$A$3:$M$45</formula>
+    <oldFormula>Disbursement!$A$3:$M$45</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="7" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Budget!$A$3:$M$21</formula>
+    <oldFormula>Budget!$A$3:$M$21</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="8" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Revenue!$A$3:$M$76</formula>
+    <oldFormula>Revenue!$A$3:$M$76</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="10" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>'Reference Tables'!$A$3:$M$140</formula>
+    <oldFormula>'Reference Tables'!$A$3:$M$140</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="11" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>'Fact Tables'!$A$3:$M$3</formula>
+    <oldFormula>'Fact Tables'!$A$3:$M$3</oldFormula>
+  </rdn>
+  <rcv guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog1611111.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rcv guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" action="delete"/>
   <rdn rId="0" localSheetId="2" customView="1" name="Z_F768F977_CCD9_4FD4_A49F_E3B56A4CB470_.wvu.FilterData" hidden="1" oldHidden="1">
@@ -11031,6 +11283,49 @@
 
 <file path=xl/revisions/revisionLog181.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcv guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Tables!$A$2:$E$89</formula>
+    <oldFormula>Tables!$A$2:$E$89</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="3" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>'Chart of Accounts'!$A$3:$M$170</formula>
+    <oldFormula>'Chart of Accounts'!$A$3:$M$170</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="4" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Vendor!$A$3:$M$45</formula>
+    <oldFormula>Vendor!$A$3:$M$45</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="5" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Contracts!$A$4:$M$159</formula>
+    <oldFormula>Contracts!$A$4:$M$159</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="6" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Disbursement!$A$3:$M$45</formula>
+    <oldFormula>Disbursement!$A$3:$M$45</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="7" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Budget!$A$3:$M$21</formula>
+    <oldFormula>Budget!$A$3:$M$21</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="8" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Revenue!$A$3:$M$76</formula>
+    <oldFormula>Revenue!$A$3:$M$76</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="10" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>'Reference Tables'!$A$3:$M$140</formula>
+    <oldFormula>'Reference Tables'!$A$3:$M$140</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="11" customView="1" name="Z_843A0AF2_4DBE_48BC_A9DB_1D590AF46394_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>'Fact Tables'!$A$3:$M$3</formula>
+    <oldFormula>'Fact Tables'!$A$3:$M$3</oldFormula>
+  </rdn>
+  <rcv guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog1811.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rcc rId="409" sId="2">
     <oc r="E73" t="inlineStr">
       <is>
@@ -11097,7 +11392,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog1811.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog18111.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rrc rId="258" sId="2" ref="A15:XFD15" action="insertRow"/>
   <rfmt sheetId="2" sqref="A15" start="0" length="0">
@@ -11367,7 +11662,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog18111.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog181111.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rfmt sheetId="1" sqref="A1:XFD7">
     <dxf>
@@ -12103,25 +12398,25 @@
     <col min="1" max="1" width="80.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="44" customFormat="1" ht="52.2" customHeight="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:1" s="45" customFormat="1" ht="52.2" customHeight="1">
+      <c r="A1" s="45" t="s">
         <v>1517</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="44" customFormat="1" ht="52.2" customHeight="1"/>
-    <row r="3" spans="1:1" s="44" customFormat="1" ht="52.2" customHeight="1"/>
-    <row r="4" spans="1:1" s="44" customFormat="1" ht="52.2" customHeight="1"/>
-    <row r="5" spans="1:1" s="44" customFormat="1" ht="52.2" customHeight="1"/>
+    <row r="2" spans="1:1" s="45" customFormat="1" ht="52.2" customHeight="1"/>
+    <row r="3" spans="1:1" s="45" customFormat="1" ht="52.2" customHeight="1"/>
+    <row r="4" spans="1:1" s="45" customFormat="1" ht="52.2" customHeight="1"/>
+    <row r="5" spans="1:1" s="45" customFormat="1" ht="52.2" customHeight="1"/>
     <row r="6" spans="1:1" s="4" customFormat="1"/>
     <row r="7" spans="1:1" s="4" customFormat="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}">
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}">
       <selection sqref="A1:XFD5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}">
+    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}">
       <selection sqref="A1:XFD5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -12159,12 +12454,12 @@
     <col min="13" max="13" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:13" s="46" customFormat="1">
+      <c r="A1" s="45" t="s">
         <v>1397</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="45" customFormat="1"/>
+    <row r="2" spans="1:13" s="46" customFormat="1"/>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>4</v>
@@ -16100,14 +16395,14 @@
   </sheetData>
   <autoFilter ref="A3:M140"/>
   <customSheetViews>
-    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" showAutoFilter="1">
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" showAutoFilter="1">
       <pane xSplit="3" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A3:M140"/>
     </customSheetView>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" showAutoFilter="1">
+    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" showAutoFilter="1">
       <pane xSplit="3" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16147,12 +16442,12 @@
     <col min="12" max="12" width="31.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:13" s="46" customFormat="1">
+      <c r="A1" s="45" t="s">
         <v>1477</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="45" customFormat="1"/>
+    <row r="2" spans="1:13" s="46" customFormat="1"/>
     <row r="3" spans="1:13" s="16" customFormat="1" ht="69">
       <c r="A3" s="13" t="s">
         <v>4</v>
@@ -16795,13 +17090,13 @@
   </sheetData>
   <autoFilter ref="A3:M25"/>
   <customSheetViews>
-    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="78" showAutoFilter="1">
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="78" showAutoFilter="1">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A3:M25"/>
     </customSheetView>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="78" showAutoFilter="1">
+    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="78" showAutoFilter="1">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16821,8 +17116,8 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E75" activeCellId="1" sqref="E73 E75"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16834,8 +17129,8 @@
     <col min="5" max="5" width="60.109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="45" customFormat="1" ht="41.4" customHeight="1">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:5" s="46" customFormat="1" ht="41.4" customHeight="1">
+      <c r="A1" s="46" t="s">
         <v>1391</v>
       </c>
     </row>
@@ -18019,7 +18314,7 @@
       <c r="D73" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E73" s="46"/>
+      <c r="E73" s="44"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="5" t="s">
@@ -18051,7 +18346,7 @@
       <c r="D75" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E75" s="46"/>
+      <c r="E75" s="44"/>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="5" t="s">
@@ -18290,19 +18585,19 @@
   </sheetData>
   <autoFilter ref="A2:E89"/>
   <customSheetViews>
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" showAutoFilter="1">
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A2:E89"/>
+    </customSheetView>
     <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" showAutoFilter="1">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E75" activeCellId="1" sqref="E73 E75"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A2:E89"/>
-    </customSheetView>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" showAutoFilter="1">
-      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A2:E72"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -18341,12 +18636,12 @@
     <col min="13" max="13" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1" ht="41.4" customHeight="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:13" s="46" customFormat="1" ht="41.4" customHeight="1">
+      <c r="A1" s="45" t="s">
         <v>1398</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="45" customFormat="1" ht="64.8" customHeight="1"/>
+    <row r="2" spans="1:13" s="46" customFormat="1" ht="64.8" customHeight="1"/>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>4</v>
@@ -23212,7 +23507,7 @@
     </filterColumn>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="75" filter="1" showAutoFilter="1">
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="75" filter="1" showAutoFilter="1">
       <pane xSplit="4" ySplit="3" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="I37" sqref="I37"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23224,7 +23519,7 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="75" filter="1" showAutoFilter="1">
+    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="75" filter="1" showAutoFilter="1">
       <pane xSplit="4" ySplit="3" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="I37" sqref="I37"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23274,12 +23569,12 @@
     <col min="14" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1" ht="14.4">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:13" s="46" customFormat="1" ht="14.4">
+      <c r="A1" s="45" t="s">
         <v>1393</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="45" customFormat="1" ht="14.4"/>
+    <row r="2" spans="1:13" s="46" customFormat="1" ht="14.4"/>
     <row r="3" spans="1:13" ht="27.6">
       <c r="A3" s="13" t="s">
         <v>4</v>
@@ -24516,13 +24811,13 @@
   </sheetData>
   <autoFilter ref="A3:M45"/>
   <customSheetViews>
-    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="73" showAutoFilter="1">
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="73" showAutoFilter="1">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A3:M45"/>
     </customSheetView>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="73" showAutoFilter="1">
+    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="73" showAutoFilter="1">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24565,13 +24860,13 @@
     <col min="13" max="13" width="27.44140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:13" s="46" customFormat="1">
+      <c r="A1" s="46" t="s">
         <v>1390</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="45" customFormat="1"/>
-    <row r="3" spans="1:13" s="45" customFormat="1" ht="57" customHeight="1"/>
+    <row r="2" spans="1:13" s="46" customFormat="1"/>
+    <row r="3" spans="1:13" s="46" customFormat="1" ht="57" customHeight="1"/>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>4</v>
@@ -29155,14 +29450,14 @@
   </sheetData>
   <autoFilter ref="A4:M159"/>
   <customSheetViews>
-    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="65" showAutoFilter="1">
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="65" showAutoFilter="1">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A4:M159"/>
     </customSheetView>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="65" showAutoFilter="1">
+    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="65" showAutoFilter="1">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -29203,12 +29498,12 @@
     <col min="13" max="13" width="19.88671875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:13" s="46" customFormat="1">
+      <c r="A1" s="45" t="s">
         <v>1396</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="45" customFormat="1"/>
+    <row r="2" spans="1:13" s="46" customFormat="1"/>
     <row r="3" spans="1:13" ht="28.8">
       <c r="A3" s="1" t="s">
         <v>4</v>
@@ -30495,13 +30790,13 @@
   </sheetData>
   <autoFilter ref="A3:M45"/>
   <customSheetViews>
-    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="75" showAutoFilter="1">
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="75" showAutoFilter="1">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A3:M45"/>
     </customSheetView>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="75" showAutoFilter="1">
+    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="75" showAutoFilter="1">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30538,12 +30833,12 @@
     <col min="13" max="13" width="21.109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:13" s="46" customFormat="1">
+      <c r="A1" s="45" t="s">
         <v>1400</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="45" customFormat="1"/>
+    <row r="2" spans="1:13" s="46" customFormat="1"/>
     <row r="3" spans="1:13" ht="28.8">
       <c r="A3" s="1" t="s">
         <v>4</v>
@@ -31122,14 +31417,14 @@
   </sheetData>
   <autoFilter ref="A3:M21"/>
   <customSheetViews>
-    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="73" showAutoFilter="1">
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="73" showAutoFilter="1">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A3:M21"/>
     </customSheetView>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="73" showAutoFilter="1">
+    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="73" showAutoFilter="1">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31174,12 +31469,12 @@
     <col min="14" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:13" s="46" customFormat="1">
+      <c r="A1" s="45" t="s">
         <v>1399</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="45" customFormat="1"/>
+    <row r="2" spans="1:13" s="46" customFormat="1"/>
     <row r="3" spans="1:13" s="26" customFormat="1" ht="27.6">
       <c r="A3" s="13" t="s">
         <v>4</v>
@@ -33231,14 +33526,14 @@
   </sheetData>
   <autoFilter ref="A3:M76"/>
   <customSheetViews>
-    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="76" showAutoFilter="1">
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="76" showAutoFilter="1">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A3:M76"/>
     </customSheetView>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="76" showAutoFilter="1">
+    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="76" showAutoFilter="1">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33278,12 +33573,12 @@
     <col min="13" max="13" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:13" s="46" customFormat="1">
+      <c r="A1" s="45" t="s">
         <v>1401</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="45" customFormat="1"/>
+    <row r="2" spans="1:13" s="46" customFormat="1"/>
     <row r="3" spans="1:13" s="16" customFormat="1" ht="27.6">
       <c r="A3" s="13" t="s">
         <v>4</v>
@@ -33686,12 +33981,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="85">
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="85">
       <selection activeCell="K7" sqref="K7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="85">
+    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="85">
       <selection activeCell="K7" sqref="K7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
NYCCHKBK-2001 wrong ticket number
git-svn-id: https://omb-dashboardplatform.reisys.com:10039/NYC_Checkbook_2_0/Database@4983 948744eb-f611-4f28-8820-250fb6d8f47d

Former-commit-id: 107feec1d633742296fd04979efd5bd0fdc8f3c2
</commit_message>
<xml_diff>
--- a/checkbook/Data Model/DataDictionary.xlsx
+++ b/checkbook/Data Model/DataDictionary.xlsx
@@ -73,10 +73,10 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Pratap Varma - Personal View" guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="855" activeSheetId="2"/>
+    <customWorkbookView name="Pratap Varma Gottumukkala - Personal View" guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="804" activeSheetId="2"/>
+    <customWorkbookView name="athiagarajan - Personal View" guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1916" windowHeight="815" activeSheetId="11"/>
     <customWorkbookView name="Kishore K. Vuppala - Personal View" guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1916" windowHeight="815" activeSheetId="1"/>
-    <customWorkbookView name="athiagarajan - Personal View" guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1916" windowHeight="815" activeSheetId="11"/>
-    <customWorkbookView name="Pratap Varma Gottumukkala - Personal View" guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1920" windowHeight="804" activeSheetId="2"/>
-    <customWorkbookView name="Pratap Varma - Personal View" guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="855" activeSheetId="10"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -7454,7 +7454,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{E5DD303C-65B6-42CE-B1C4-D442DB814DE0}" diskRevisions="1" revisionId="4" version="3">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A6187A50-8DA9-4D79-8E67-E7C401C0E25B}" diskRevisions="1" revisionId="14" version="4">
   <header guid="{C99DDCD8-9C3B-4B35-A46B-11BEE8D90BCF}" dateTime="2012-12-13T14:56:59" maxSheetId="13" userName="Pratap Varma" r:id="rId1">
     <sheetIdMap count="12">
       <sheetId val="1"/>
@@ -7488,6 +7488,22 @@
     </sheetIdMap>
   </header>
   <header guid="{E5DD303C-65B6-42CE-B1C4-D442DB814DE0}" dateTime="2012-12-13T16:27:19" maxSheetId="13" userName="Pratap Varma" r:id="rId3" minRId="2" maxRId="4">
+    <sheetIdMap count="12">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="9"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A6187A50-8DA9-4D79-8E67-E7C401C0E25B}" dateTime="2012-12-13T19:31:26" maxSheetId="13" userName="Pratap Varma" r:id="rId4">
     <sheetIdMap count="12">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -7711,8 +7727,57 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_00C7CAED_15A0_4F6F_B460_E637CABE0590_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Tables!$A$2:$F$95</formula>
+    <oldFormula>Tables!$A$2:$F$95</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="3" customView="1" name="Z_00C7CAED_15A0_4F6F_B460_E637CABE0590_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>'Chart of Accounts'!$A$3:$M$3</formula>
+    <oldFormula>'Chart of Accounts'!$A$3:$M$3</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="4" customView="1" name="Z_00C7CAED_15A0_4F6F_B460_E637CABE0590_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Vendor!$A$3:$M$3</formula>
+    <oldFormula>Vendor!$A$3:$M$3</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="5" customView="1" name="Z_00C7CAED_15A0_4F6F_B460_E637CABE0590_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Contracts!$A$4:$M$258</formula>
+    <oldFormula>Contracts!$A$4:$M$258</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="6" customView="1" name="Z_00C7CAED_15A0_4F6F_B460_E637CABE0590_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Disbursement!$A$3:$M$57</formula>
+    <oldFormula>Disbursement!$A$3:$M$57</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="7" customView="1" name="Z_00C7CAED_15A0_4F6F_B460_E637CABE0590_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Budget!$A$3:$M$35</formula>
+    <oldFormula>Budget!$A$3:$M$35</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="8" customView="1" name="Z_00C7CAED_15A0_4F6F_B460_E637CABE0590_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Revenue!$A$3:$M$77</formula>
+    <oldFormula>Revenue!$A$3:$M$77</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="9" customView="1" name="Z_00C7CAED_15A0_4F6F_B460_E637CABE0590_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Payroll!$A$3:$M$81</formula>
+    <oldFormula>Payroll!$A$3:$M$81</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="10" customView="1" name="Z_00C7CAED_15A0_4F6F_B460_E637CABE0590_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>'Reference Tables'!$A$3:$M$92</formula>
+    <oldFormula>'Reference Tables'!$A$3:$M$92</oldFormula>
+  </rdn>
+  <rdn rId="0" localSheetId="11" customView="1" name="Z_00C7CAED_15A0_4F6F_B460_E637CABE0590_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>'Fact Tables'!$A$3:$M$390</formula>
+    <oldFormula>'Fact Tables'!$A$3:$M$390</oldFormula>
+  </rdn>
+  <rcv guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{A6187A50-8DA9-4D79-8E67-E7C401C0E25B}" name="Pratap Varma" id="-279991011" dateTime="2012-12-13T19:31:15"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8026,22 +8091,22 @@
     <row r="7" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}">
+    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}">
       <selection sqref="A1:XFD5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}">
+    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}">
       <selection sqref="A1:XFD5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}">
+    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}">
       <selection sqref="A1:XFD5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}">
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}">
       <selection sqref="A1:XFD5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
@@ -10613,31 +10678,31 @@
   </sheetData>
   <autoFilter ref="A3:M92"/>
   <customSheetViews>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" showAutoFilter="1">
-      <pane xSplit="3" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
+      <selection sqref="A1:XFD2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A3:M140"/>
+      <autoFilter ref="A3:M92"/>
+    </customSheetView>
+    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}">
+      <pane xSplit="3" ySplit="3" topLeftCell="D82" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B90" sqref="B90"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" showAutoFilter="1">
       <pane xSplit="3" ySplit="3" topLeftCell="D80" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="I83" sqref="I83"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
+      <pageSetup orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A3:M158"/>
     </customSheetView>
-    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}">
-      <pane xSplit="3" ySplit="3" topLeftCell="D82" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B90" sqref="B90"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId3"/>
-    </customSheetView>
-    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
-      <selection sqref="A1:XFD2"/>
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" showAutoFilter="1">
+      <pane xSplit="3" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A3:M92"/>
+      <autoFilter ref="A3:M140"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -36934,11 +36999,18 @@
   </sheetData>
   <autoFilter ref="A3:M390"/>
   <customSheetViews>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="78" showAutoFilter="1">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
+      <selection sqref="A1:XFD2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A3:M25"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A3:M390"/>
+    </customSheetView>
+    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="78" showAutoFilter="1">
+      <pane xSplit="4" ySplit="3" topLeftCell="E184" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B207" sqref="B207"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A3:XFD343"/>
     </customSheetView>
     <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" showAutoFilter="1">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
@@ -36946,18 +37018,11 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A3:M130"/>
     </customSheetView>
-    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="78" showAutoFilter="1">
-      <pane xSplit="4" ySplit="3" topLeftCell="E184" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B207" sqref="B207"/>
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="78" showAutoFilter="1">
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A3:XFD343"/>
-    </customSheetView>
-    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
-      <selection sqref="A1:XFD2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A3:M390"/>
+      <autoFilter ref="A3:M25"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -36979,15 +37044,15 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <customSheetViews>
-    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}">
+    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" state="hidden">
+      <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" state="hidden">
       <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" state="hidden">
-      <selection activeCell="A3" sqref="A3"/>
+    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -37000,7 +37065,8 @@
   <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <pane ySplit="95" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38582,39 +38648,33 @@
   </sheetData>
   <autoFilter ref="A2:F95"/>
   <customSheetViews>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" showAutoFilter="1">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
+      <pane ySplit="94" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A2:E89"/>
+      <autoFilter ref="A2:F95"/>
+    </customSheetView>
+    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" showAutoFilter="1">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A2:F123"/>
     </customSheetView>
     <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" showAutoFilter="1">
       <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
+      <pageSetup orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A2:E100"/>
     </customSheetView>
-    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" showAutoFilter="1">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:F123"/>
-    </customSheetView>
-    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" filter="1" showAutoFilter="1">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" showAutoFilter="1">
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A2:F96">
-        <filterColumn colId="0">
-          <filters>
-            <filter val="ref_data_source"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
+      <autoFilter ref="A2:E89"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -44223,6 +44283,22 @@
   </sheetData>
   <autoFilter ref="A3:M197"/>
   <customSheetViews>
+    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
+      <selection sqref="A1:XFD2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A3:M197"/>
+    </customSheetView>
+    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="75" topLeftCell="A181">
+      <selection activeCell="B202" sqref="B202"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="75" showAutoFilter="1">
+      <pane xSplit="4" ySplit="4" topLeftCell="E176" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="F184" sqref="F184"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A3:M184"/>
+    </customSheetView>
     <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="75" filter="1" showAutoFilter="1">
       <pane xSplit="4" ySplit="3" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="I37" sqref="I37"/>
@@ -44234,22 +44310,6 @@
           </filters>
         </filterColumn>
       </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="75" showAutoFilter="1">
-      <pane xSplit="4" ySplit="4" topLeftCell="E176" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F184" sqref="F184"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A3:M184"/>
-    </customSheetView>
-    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="75" topLeftCell="A181">
-      <selection activeCell="B202" sqref="B202"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
-      <selection sqref="A1:XFD2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A3:M3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -45615,11 +45675,16 @@
   </sheetData>
   <autoFilter ref="A3:M47"/>
   <customSheetViews>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="73" showAutoFilter="1">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
+    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
+      <selection sqref="A1:XFD2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A3:M45"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A3:M47"/>
+    </customSheetView>
+    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="73" showAutoFilter="1" topLeftCell="A18">
+      <selection activeCell="E35" sqref="E35:K35"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A3:M47"/>
     </customSheetView>
     <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" showAutoFilter="1">
       <pane xSplit="3" ySplit="3" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
@@ -45627,16 +45692,11 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A3:M47"/>
     </customSheetView>
-    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="73" showAutoFilter="1" topLeftCell="A18">
-      <selection activeCell="E35" sqref="E35:K35"/>
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="73" showAutoFilter="1">
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A3:M47"/>
-    </customSheetView>
-    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
-      <selection sqref="A1:XFD2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A3:M47"/>
+      <autoFilter ref="A3:M45"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -52800,32 +52860,32 @@
   </sheetData>
   <autoFilter ref="A4:M258"/>
   <customSheetViews>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="65" showAutoFilter="1">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
+    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
+      <selection sqref="A1:XFD3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A4:M159"/>
+      <autoFilter ref="A4:M258"/>
+    </customSheetView>
+    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="65" showAutoFilter="1">
+      <pane xSplit="3" ySplit="4" topLeftCell="D191" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B207" sqref="B207:B209"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A4:M311"/>
     </customSheetView>
     <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" showAutoFilter="1">
       <pane xSplit="3" ySplit="4" topLeftCell="E50" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="A57" sqref="A57:XFD59"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
+      <pageSetup orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A4:M163"/>
     </customSheetView>
-    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="65" showAutoFilter="1">
-      <pane xSplit="3" ySplit="4" topLeftCell="D191" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B207" sqref="B207:B209"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A4:M311"/>
-    </customSheetView>
-    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
-      <selection sqref="A1:XFD3"/>
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="65" showAutoFilter="1">
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A4:M258"/>
+      <autoFilter ref="A4:M159"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -54455,11 +54515,15 @@
   </sheetData>
   <autoFilter ref="A3:M57"/>
   <customSheetViews>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="75" showAutoFilter="1">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
+      <selection sqref="A1:XFD2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A3:M45"/>
+      <autoFilter ref="A3:M57"/>
+    </customSheetView>
+    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="80" showAutoFilter="1" topLeftCell="A42">
+      <selection activeCell="A53" sqref="A53"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A3:M55"/>
     </customSheetView>
     <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" showAutoFilter="1">
       <pane xSplit="3" ySplit="3" topLeftCell="D31" activePane="bottomRight" state="frozen"/>
@@ -54467,15 +54531,11 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A3:M48"/>
     </customSheetView>
-    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="80" showAutoFilter="1" topLeftCell="A42">
-      <selection activeCell="A53" sqref="A53"/>
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="75" showAutoFilter="1">
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A3:M55"/>
-    </customSheetView>
-    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
-      <selection sqref="A1:XFD2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A3:M57"/>
+      <autoFilter ref="A3:M45"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -56209,30 +56269,30 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="73" showAutoFilter="1">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}">
+      <selection sqref="A1:XFD2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A3:M21"/>
+    </customSheetView>
+    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="73">
+      <pane xSplit="4" ySplit="3" topLeftCell="E39" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E44" sqref="E44"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="73" showAutoFilter="1">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
+      <pageSetup orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A3:M32"/>
     </customSheetView>
-    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="73">
-      <pane xSplit="4" ySplit="3" topLeftCell="E39" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E44" sqref="E44"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId3"/>
-    </customSheetView>
-    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}">
-      <selection sqref="A1:XFD2"/>
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="73" showAutoFilter="1">
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
+      <autoFilter ref="A3:M21"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -58504,32 +58564,32 @@
   </sheetData>
   <autoFilter ref="A3:M77"/>
   <customSheetViews>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="76" showAutoFilter="1">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
+      <selection sqref="A1:XFD2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A3:M76"/>
+      <autoFilter ref="A3:M77"/>
+    </customSheetView>
+    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="75" showAutoFilter="1">
+      <pane xSplit="4" ySplit="3" topLeftCell="E63" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A85" sqref="A85"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A3:M77"/>
     </customSheetView>
     <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="76" showAutoFilter="1">
       <pane xSplit="4" ySplit="3" topLeftCell="E67" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="L76" sqref="L76"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
+      <pageSetup orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A3:M78"/>
     </customSheetView>
-    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="75" showAutoFilter="1">
-      <pane xSplit="4" ySplit="3" topLeftCell="E63" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A85" sqref="A85"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A3:M77"/>
-    </customSheetView>
-    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}" showAutoFilter="1">
-      <selection sqref="A1:XFD2"/>
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="76" showAutoFilter="1">
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A3:M77"/>
+      <autoFilter ref="A3:M76"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -60641,23 +60701,23 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="85">
-      <selection activeCell="K7" sqref="K7"/>
+    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}">
+      <selection sqref="A1:XFD2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="85" topLeftCell="A59">
+      <selection activeCell="A82" sqref="A82"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{843A0AF2-4DBE-48BC-A9DB-1D590AF46394}" scale="85">
       <selection activeCell="K7" sqref="K7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{7A86E65E-CCCB-4C01-8F2E-D18114648424}" scale="85" topLeftCell="A59">
-      <selection activeCell="A82" sqref="A82"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{00C7CAED-15A0-4F6F-B460-E637CABE0590}">
-      <selection sqref="A1:XFD2"/>
+    <customSheetView guid="{F768F977-CCD9-4FD4-A49F-E3B56A4CB470}" scale="85">
+      <selection activeCell="K7" sqref="K7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>

</xml_diff>